<commit_message>
Add the RTSL type codes to the benchmarks fixture
</commit_message>
<xml_diff>
--- a/data/RTSL Fixtures.xlsx
+++ b/data/RTSL Fixtures.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/savanni/src/cloud-city/rtsl-benchmarks/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{365580E7-1F74-F345-B44A-8F11F64C6FC4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440E6AC8-5F3C-1048-BB66-2DAA3418FD50}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Benchmark Capacities" sheetId="1" r:id="rId1"/>
     <sheet name="Activities" sheetId="2" r:id="rId2"/>
     <sheet name="Crosswalk" sheetId="3" r:id="rId3"/>
-    <sheet name="SPAR 2018" sheetId="4" r:id="rId4"/>
-    <sheet name="JEE 1" sheetId="5" r:id="rId5"/>
-    <sheet name="JEE 2" sheetId="6" r:id="rId6"/>
+    <sheet name="Type Codes" sheetId="7" r:id="rId4"/>
+    <sheet name="SPAR 2018" sheetId="4" r:id="rId5"/>
+    <sheet name="JEE 1" sheetId="5" r:id="rId6"/>
+    <sheet name="JEE 2" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1483" uniqueCount="1176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1516" uniqueCount="1207">
   <si>
     <t>JEE2 Capacity</t>
   </si>
@@ -3695,12 +3696,106 @@
   <si>
     <t>Develop and conduct emergency response drills and other exercises on radiation emergency and update the response plan, mechanisms and guidelines accordingly.</t>
   </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1
+</t>
+  </si>
+  <si>
+    <t>Advocacy</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Assessment and Data Use</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Coordination</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Designation</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Dissemination</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Financing</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Monitoring and Evaluation</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Planning and Strategy</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Procurement</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Program Implementation</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>SimEx and AAR</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>SOPs</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>Tool Development</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -3717,16 +3812,34 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -3734,11 +3847,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3748,6 +3876,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3968,7 +4102,7 @@
   </sheetPr>
   <dimension ref="A1:E1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -24326,7 +24460,9 @@
   </sheetPr>
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -26687,6 +26823,197 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC24E058-E931-ED46-8CAB-042C21967DFC}">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" s="9" t="s">
+        <v>1176</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1177</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+      <c r="A2" s="9">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>1178</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+      <c r="A3" s="9">
+        <v>1</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>1180</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>1181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+      <c r="A4" s="9">
+        <v>1</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>1182</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A5" s="9">
+        <v>1</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>1184</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+      <c r="A6" s="9">
+        <v>1</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>1186</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A7" s="9">
+        <v>1</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>1188</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>1189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="48" x14ac:dyDescent="0.15">
+      <c r="A8" s="9">
+        <v>1</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>1190</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+      <c r="A9" s="9">
+        <v>1</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+      <c r="A10" s="9">
+        <v>1</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>1194</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="48" x14ac:dyDescent="0.15">
+      <c r="A11" s="9">
+        <v>1</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>1196</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+      <c r="A12" s="9">
+        <v>1</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>1198</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A13" s="9">
+        <v>1</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>1200</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A14" s="9">
+        <v>1</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>1202</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="48" x14ac:dyDescent="0.15">
+      <c r="A15" s="9">
+        <v>1</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>1203</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>1204</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A16" s="9">
+        <v>1</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>1205</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>1206</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B1000"/>
   <sheetViews>
@@ -27878,7 +28205,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -28286,7 +28613,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>

</xml_diff>